<commit_message>
Use raw SayCan prompt
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c7a197fbcb7db713/Documents/School/CS 638/Project/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="388" documentId="8_{F81DD993-C52C-644A-A6B1-063746E280F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63CA22C2-3382-7546-BEFB-137DA7BE031A}"/>
+  <xr:revisionPtr revIDLastSave="452" documentId="8_{F81DD993-C52C-644A-A6B1-063746E280F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CA83465-1A20-D447-B932-ECBB4CFD4FA5}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="18020" xr2:uid="{579ECF8A-8911-314F-B702-462A636067A9}"/>
   </bookViews>
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BD652BF-F26B-4E40-BDF4-D987A03C2729}">
   <dimension ref="A1:AA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="B2:Y3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,10 +604,136 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">

</xml_diff>